<commit_message>
oprydning og forberedelse af 2021-22
</commit_message>
<xml_diff>
--- a/adm/2020-21/Byrdefordeling.xlsx
+++ b/adm/2020-21/Byrdefordeling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP/adm/2020-21/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrh630/repositories/PoP.git/adm/2020-21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53B2B91-EB5A-A44E-B177-80C36FBBEEC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D36244-27B6-E443-9DFF-7880C7C55814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33160" yWindow="460" windowWidth="21060" windowHeight="6940" xr2:uid="{C7745739-1061-4147-B11C-6224BC72E703}"/>
+    <workbookView xWindow="15340" yWindow="8380" windowWidth="23060" windowHeight="15620" xr2:uid="{C7745739-1061-4147-B11C-6224BC72E703}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Teaching hours</t>
   </si>
   <si>
-    <t>Lectures</t>
-  </si>
-  <si>
     <t>Present teaching hours</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Afrunding</t>
+  </si>
+  <si>
+    <t>Weeks</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,24 +454,24 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <f>D2/D5</f>

</xml_diff>